<commit_message>
Some PHY control added
</commit_message>
<xml_diff>
--- a/SVD_Files/Ethernet.xlsx
+++ b/SVD_Files/Ethernet.xlsx
@@ -719,9 +719,6 @@
   </si>
   <si>
     <t>1: Send preambula (0xFFFFFFFF), 0: No preambula</t>
-  </si>
-  <si>
-    <t>0: read, 1: write</t>
   </si>
   <si>
     <t>PHY address on MDIO bus</t>
@@ -1293,6 +1290,9 @@
   </si>
   <si>
     <t>0x3F00</t>
+  </si>
+  <si>
+    <t>1: read, 0: write</t>
   </si>
 </sst>
 </file>
@@ -1895,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:AL265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3328,7 +3328,7 @@
     <row r="108" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
       <c r="B108" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>5</v>
@@ -3608,7 +3608,7 @@
     <row r="129" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
       <c r="B129" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C129" s="8" t="s">
         <v>4</v>
@@ -3617,7 +3617,7 @@
     <row r="130" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
       <c r="B130" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C130" s="8" t="s">
         <v>5</v>
@@ -3672,10 +3672,10 @@
         <v>184</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="135" spans="1:38" x14ac:dyDescent="0.25">
@@ -3686,7 +3686,7 @@
         <v>187</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="136" spans="1:38" x14ac:dyDescent="0.25">
@@ -3697,7 +3697,7 @@
         <v>188</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="137" spans="1:38" x14ac:dyDescent="0.25">
@@ -3708,7 +3708,7 @@
         <v>189</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>193</v>
+        <v>355</v>
       </c>
     </row>
     <row r="138" spans="1:38" x14ac:dyDescent="0.25">
@@ -3736,7 +3736,7 @@
     <row r="140" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A140" s="5"/>
       <c r="B140" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C140" s="8" t="s">
         <v>4</v>
@@ -3753,10 +3753,10 @@
     </row>
     <row r="144" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C144" s="2"/>
       <c r="D144"/>
@@ -3800,16 +3800,16 @@
         <v>1</v>
       </c>
       <c r="B145" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C145" s="5" t="s">
         <v>200</v>
-      </c>
-      <c r="C145" s="5" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="146" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
       <c r="B146" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C146" s="8" t="s">
         <v>4</v>
@@ -3826,13 +3826,13 @@
     </row>
     <row r="150" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D150"/>
       <c r="E150"/>
@@ -3872,10 +3872,10 @@
     </row>
     <row r="151" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C151" s="15" t="s">
         <v>6</v>
@@ -3918,13 +3918,13 @@
     </row>
     <row r="152" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C152" s="36" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D152"/>
       <c r="E152"/>
@@ -3964,13 +3964,13 @@
     </row>
     <row r="153" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C153" s="36" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D153"/>
       <c r="E153"/>
@@ -4013,16 +4013,16 @@
         <v>1</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="155" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A155" s="5"/>
       <c r="B155" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C155" s="8" t="s">
         <v>4</v>
@@ -4039,10 +4039,10 @@
     </row>
     <row r="159" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B159" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="C159" s="2"/>
       <c r="D159"/>
@@ -4086,10 +4086,10 @@
         <v>0</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="161" spans="1:38" x14ac:dyDescent="0.25">
@@ -4097,10 +4097,10 @@
         <v>1</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="162" spans="1:38" x14ac:dyDescent="0.25">
@@ -4108,10 +4108,10 @@
         <v>2</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="163" spans="1:38" x14ac:dyDescent="0.25">
@@ -4119,10 +4119,10 @@
         <v>3</v>
       </c>
       <c r="B163" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="164" spans="1:38" x14ac:dyDescent="0.25">
@@ -4130,10 +4130,10 @@
         <v>4</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="165" spans="1:38" x14ac:dyDescent="0.25">
@@ -4141,10 +4141,10 @@
         <v>185</v>
       </c>
       <c r="B165" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C165" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="C165" s="5" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="166" spans="1:38" x14ac:dyDescent="0.25">
@@ -4152,10 +4152,10 @@
         <v>8</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="167" spans="1:38" x14ac:dyDescent="0.25">
@@ -4163,10 +4163,10 @@
         <v>9</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="168" spans="1:38" x14ac:dyDescent="0.25">
@@ -4174,10 +4174,10 @@
         <v>10</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="169" spans="1:38" x14ac:dyDescent="0.25">
@@ -4185,10 +4185,10 @@
         <v>11</v>
       </c>
       <c r="B169" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="170" spans="1:38" x14ac:dyDescent="0.25">
@@ -4196,16 +4196,16 @@
         <v>12</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="171" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A171" s="5"/>
       <c r="B171" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C171" s="8" t="s">
         <v>4</v>
@@ -4214,7 +4214,7 @@
     <row r="172" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A172" s="5"/>
       <c r="B172" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C172" s="8" t="s">
         <v>5</v>
@@ -4222,13 +4222,13 @@
     </row>
     <row r="175" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B175" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C175" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D175"/>
       <c r="E175"/>
@@ -4271,82 +4271,82 @@
         <v>0</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="13"/>
       <c r="B178" s="5"/>
       <c r="C178" s="21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="13"/>
       <c r="B179" s="5"/>
       <c r="C179" s="21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="13"/>
       <c r="B180" s="5"/>
       <c r="C180" s="21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="13"/>
       <c r="B181" s="5"/>
       <c r="C181" s="21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="13"/>
       <c r="B182" s="5"/>
       <c r="C182" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="13"/>
       <c r="B183" s="5"/>
       <c r="C183" s="21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="13"/>
       <c r="B184" s="5"/>
       <c r="C184" s="21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="13"/>
       <c r="B185" s="5"/>
       <c r="C185" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B186" s="11" t="s">
         <v>75</v>
@@ -4358,10 +4358,10 @@
         <v>7</v>
       </c>
       <c r="B187" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -4369,10 +4369,10 @@
         <v>8</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -4380,10 +4380,10 @@
         <v>9</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C189" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -4391,27 +4391,27 @@
         <v>10</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="5"/>
       <c r="B192" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C192" s="8" t="s">
         <v>4</v>
@@ -4420,7 +4420,7 @@
     <row r="193" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A193" s="5"/>
       <c r="B193" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C193" s="8" t="s">
         <v>5</v>
@@ -4428,13 +4428,13 @@
     </row>
     <row r="196" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B196" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C196" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D196"/>
       <c r="E196"/>
@@ -4477,10 +4477,10 @@
         <v>0</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C197" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="198" spans="1:38" x14ac:dyDescent="0.25">
@@ -4488,10 +4488,10 @@
         <v>1</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C198" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="199" spans="1:38" x14ac:dyDescent="0.25">
@@ -4499,10 +4499,10 @@
         <v>2</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C199" s="21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="200" spans="1:38" x14ac:dyDescent="0.25">
@@ -4510,10 +4510,10 @@
         <v>3</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C200" s="21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="201" spans="1:38" x14ac:dyDescent="0.25">
@@ -4521,10 +4521,10 @@
         <v>4</v>
       </c>
       <c r="B201" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C201" s="21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="202" spans="1:38" x14ac:dyDescent="0.25">
@@ -4532,21 +4532,21 @@
         <v>5</v>
       </c>
       <c r="B202" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C202" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="203" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A203" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B203" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C203" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="204" spans="1:38" x14ac:dyDescent="0.25">
@@ -4554,10 +4554,10 @@
         <v>8</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C204" s="21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="205" spans="1:38" x14ac:dyDescent="0.25">
@@ -4565,10 +4565,10 @@
         <v>9</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C205" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="206" spans="1:38" x14ac:dyDescent="0.25">
@@ -4576,16 +4576,16 @@
         <v>10</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C206" s="21" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="207" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A207" s="5"/>
       <c r="B207" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C207" s="8" t="s">
         <v>4</v>
@@ -4594,7 +4594,7 @@
     <row r="208" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A208" s="5"/>
       <c r="B208" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C208" s="8" t="s">
         <v>5</v>
@@ -4602,13 +4602,13 @@
     </row>
     <row r="212" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B212" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C212" s="18" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D212"/>
       <c r="E212"/>
@@ -4651,16 +4651,16 @@
         <v>1</v>
       </c>
       <c r="B213" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C213" s="5" t="s">
         <v>241</v>
-      </c>
-      <c r="C213" s="5" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="214" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A214" s="5"/>
       <c r="B214" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C214" s="8" t="s">
         <v>4</v>
@@ -4677,13 +4677,13 @@
     </row>
     <row r="218" spans="1:38" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B218" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C218" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D218" s="23"/>
       <c r="E218" s="23"/>
@@ -4726,10 +4726,10 @@
         <v>0</v>
       </c>
       <c r="B219" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C219" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="220" spans="1:38" x14ac:dyDescent="0.25">
@@ -4740,7 +4740,7 @@
         <v>114</v>
       </c>
       <c r="C220" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="221" spans="1:38" x14ac:dyDescent="0.25">
@@ -4748,10 +4748,10 @@
         <v>2</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C221" s="21" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="222" spans="1:38" x14ac:dyDescent="0.25">
@@ -4759,10 +4759,10 @@
         <v>3</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C222" s="21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="223" spans="1:38" x14ac:dyDescent="0.25">
@@ -4770,10 +4770,10 @@
         <v>4</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C223" s="21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="224" spans="1:38" x14ac:dyDescent="0.25">
@@ -4781,21 +4781,21 @@
         <v>5</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C224" s="21" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="225" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A225" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C225" s="21" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="226" spans="1:38" x14ac:dyDescent="0.25">
@@ -4815,7 +4815,7 @@
         <v>122</v>
       </c>
       <c r="C227" s="21" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="228" spans="1:38" x14ac:dyDescent="0.25">
@@ -4823,16 +4823,16 @@
         <v>15</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C228" s="21" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="229" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A229" s="5"/>
       <c r="B229" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C229" s="8" t="s">
         <v>4</v>
@@ -4841,7 +4841,7 @@
     <row r="230" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A230" s="5"/>
       <c r="B230" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C230" s="8" t="s">
         <v>5</v>
@@ -4849,13 +4849,13 @@
     </row>
     <row r="233" spans="1:38" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A233" s="22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B233" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C233" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D233" s="23"/>
       <c r="E233" s="23"/>
@@ -4907,10 +4907,10 @@
         <v>8</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C235" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="236" spans="1:38" x14ac:dyDescent="0.25">
@@ -4918,10 +4918,10 @@
         <v>9</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C236" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="237" spans="1:38" x14ac:dyDescent="0.25">
@@ -4929,10 +4929,10 @@
         <v>10</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C237" s="21" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="238" spans="1:38" x14ac:dyDescent="0.25">
@@ -4940,10 +4940,10 @@
         <v>11</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C238" s="21" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="239" spans="1:38" x14ac:dyDescent="0.25">
@@ -4951,10 +4951,10 @@
         <v>12</v>
       </c>
       <c r="B239" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C239" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="240" spans="1:38" x14ac:dyDescent="0.25">
@@ -4962,16 +4962,16 @@
         <v>13</v>
       </c>
       <c r="B240" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C240" s="21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="241" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A241" s="5"/>
       <c r="B241" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C241" s="8" t="s">
         <v>4</v>
@@ -4980,7 +4980,7 @@
     <row r="242" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A242" s="5"/>
       <c r="B242" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C242" s="8" t="s">
         <v>5</v>
@@ -4988,13 +4988,13 @@
     </row>
     <row r="245" spans="1:38" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A245" s="22" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B245" s="18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C245" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D245" s="23"/>
       <c r="E245" s="23"/>
@@ -5037,46 +5037,46 @@
         <v>0</v>
       </c>
       <c r="B246" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C246" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="247" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A247" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B247" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C247" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="248" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A248" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B248" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C248" s="21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="249" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A249" s="13"/>
       <c r="B249" s="5"/>
       <c r="C249" s="21" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="250" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A250" s="13"/>
       <c r="B250" s="5"/>
       <c r="C250" s="21" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="251" spans="1:38" x14ac:dyDescent="0.25">
@@ -5093,10 +5093,10 @@
         <v>14</v>
       </c>
       <c r="B252" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C252" s="21" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="253" spans="1:38" x14ac:dyDescent="0.25">
@@ -5104,16 +5104,16 @@
         <v>15</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C253" s="21" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="254" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A254" s="5"/>
       <c r="B254" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C254" s="8" t="s">
         <v>4</v>
@@ -5122,7 +5122,7 @@
     <row r="255" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A255" s="5"/>
       <c r="B255" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C255" s="8" t="s">
         <v>5</v>
@@ -5131,61 +5131,61 @@
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="29"/>
       <c r="B260" s="32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C260" s="31"/>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B261" s="30" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C261" s="31" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="34" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B262" s="25" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C262" s="26" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="35"/>
       <c r="B263" s="27" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C263" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="33" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B264" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="C264" s="31" t="s">
         <v>343</v>
-      </c>
-      <c r="C264" s="31" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="33" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B265" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="C265" s="31" t="s">
         <v>343</v>
-      </c>
-      <c r="C265" s="31" t="s">
-        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>